<commit_message>
Change privileges of storeman and add create tent from template
</commit_message>
<xml_diff>
--- a/public/docs/vykaz_na_akciu_NEW.xlsx
+++ b/public/docs/vykaz_na_akciu_NEW.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MiHu\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MiHu\Documents\projects\is-klost\is-klost\public\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Hárok2" sheetId="2" r:id="rId2"/>
     <sheet name="Hárok3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -762,63 +762,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
@@ -850,15 +802,63 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -880,16 +880,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>590550</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>200025</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>819150</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -913,7 +913,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="85725" y="57150"/>
+          <a:off x="2686050" y="666750"/>
           <a:ext cx="504825" cy="142875"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1239,7 +1239,7 @@
   <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1254,84 +1254,84 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
       <c r="H1" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="52" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="53"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="55" t="s">
+      <c r="B2" s="79"/>
+      <c r="C2" s="79"/>
+      <c r="D2" s="80"/>
+      <c r="E2" s="81" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="53"/>
-      <c r="G2" s="53"/>
-      <c r="H2" s="56"/>
+      <c r="F2" s="79"/>
+      <c r="G2" s="79"/>
+      <c r="H2" s="82"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="58"/>
-      <c r="C3" s="58"/>
-      <c r="D3" s="59"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="58"/>
-      <c r="G3" s="58"/>
-      <c r="H3" s="61"/>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="40"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="41"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="58"/>
-      <c r="C4" s="58"/>
-      <c r="D4" s="59"/>
-      <c r="E4" s="60"/>
-      <c r="F4" s="58"/>
-      <c r="G4" s="58"/>
-      <c r="H4" s="61"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="40"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="41"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="72" t="s">
+      <c r="A5" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="74"/>
-      <c r="E5" s="78" t="s">
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="54"/>
+      <c r="E5" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="79"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="59"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="77"/>
-      <c r="E6" s="80" t="s">
+      <c r="B6" s="56"/>
+      <c r="C6" s="56"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="81"/>
-      <c r="G6" s="81"/>
-      <c r="H6" s="82"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="34"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
@@ -1339,10 +1339,10 @@
       </c>
       <c r="B7" s="18"/>
       <c r="C7" s="18"/>
-      <c r="D7" s="50" t="s">
+      <c r="D7" s="76" t="s">
         <v>33</v>
       </c>
-      <c r="E7" s="51"/>
+      <c r="E7" s="77"/>
       <c r="F7" s="30" t="s">
         <v>34</v>
       </c>
@@ -1350,38 +1350,38 @@
       <c r="H7" s="20"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="41"/>
-      <c r="C8" s="44" t="s">
+      <c r="B8" s="65"/>
+      <c r="C8" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="45"/>
-      <c r="E8" s="46"/>
-      <c r="F8" s="42" t="s">
+      <c r="D8" s="69"/>
+      <c r="E8" s="70"/>
+      <c r="F8" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="G8" s="83" t="s">
+      <c r="G8" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="38" t="s">
+      <c r="H8" s="62" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="40"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="47"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="49"/>
-      <c r="F9" s="43"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="39"/>
+      <c r="A9" s="64"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="67"/>
+      <c r="G9" s="36"/>
+      <c r="H9" s="63"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="32"/>
-      <c r="B10" s="33"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="61"/>
       <c r="C10" s="9"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -1390,8 +1390,8 @@
       <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="32"/>
-      <c r="B11" s="33"/>
+      <c r="A11" s="60"/>
+      <c r="B11" s="61"/>
       <c r="C11" s="9"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
@@ -1400,8 +1400,8 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="32"/>
-      <c r="B12" s="33"/>
+      <c r="A12" s="60"/>
+      <c r="B12" s="61"/>
       <c r="C12" s="9"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
@@ -1410,8 +1410,8 @@
       <c r="H12" s="13"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="32"/>
-      <c r="B13" s="33"/>
+      <c r="A13" s="60"/>
+      <c r="B13" s="61"/>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
@@ -1420,8 +1420,8 @@
       <c r="H13" s="13"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="32"/>
-      <c r="B14" s="33"/>
+      <c r="A14" s="60"/>
+      <c r="B14" s="61"/>
       <c r="C14" s="9"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1430,8 +1430,8 @@
       <c r="H14" s="13"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="32"/>
-      <c r="B15" s="33"/>
+      <c r="A15" s="60"/>
+      <c r="B15" s="61"/>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
@@ -1440,8 +1440,8 @@
       <c r="H15" s="13"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="32"/>
-      <c r="B16" s="33"/>
+      <c r="A16" s="60"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="9"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
@@ -1450,8 +1450,8 @@
       <c r="H16" s="13"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="32"/>
-      <c r="B17" s="33"/>
+      <c r="A17" s="60"/>
+      <c r="B17" s="61"/>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
       <c r="E17" s="8"/>
@@ -1460,8 +1460,8 @@
       <c r="H17" s="13"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="61"/>
       <c r="C18" s="9"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
@@ -1470,8 +1470,8 @@
       <c r="H18" s="13"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="32"/>
-      <c r="B19" s="33"/>
+      <c r="A19" s="60"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="7"/>
       <c r="D19" s="8"/>
       <c r="E19" s="8"/>
@@ -1480,8 +1480,8 @@
       <c r="H19" s="13"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="32"/>
-      <c r="B20" s="33"/>
+      <c r="A20" s="60"/>
+      <c r="B20" s="61"/>
       <c r="C20" s="9"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1490,8 +1490,8 @@
       <c r="H20" s="13"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="32"/>
-      <c r="B21" s="33"/>
+      <c r="A21" s="60"/>
+      <c r="B21" s="61"/>
       <c r="C21" s="7"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
@@ -1500,8 +1500,8 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="32"/>
-      <c r="B22" s="33"/>
+      <c r="A22" s="60"/>
+      <c r="B22" s="61"/>
       <c r="C22" s="9"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1510,8 +1510,8 @@
       <c r="H22" s="13"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="32"/>
-      <c r="B23" s="33"/>
+      <c r="A23" s="60"/>
+      <c r="B23" s="61"/>
       <c r="C23" s="9"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1520,8 +1520,8 @@
       <c r="H23" s="13"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="32"/>
-      <c r="B24" s="33"/>
+      <c r="A24" s="60"/>
+      <c r="B24" s="61"/>
       <c r="C24" s="3"/>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
@@ -1530,8 +1530,8 @@
       <c r="H24" s="13"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="32"/>
-      <c r="B25" s="33"/>
+      <c r="A25" s="60"/>
+      <c r="B25" s="61"/>
       <c r="C25" s="9"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1540,8 +1540,8 @@
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="32"/>
-      <c r="B26" s="33"/>
+      <c r="A26" s="60"/>
+      <c r="B26" s="61"/>
       <c r="C26" s="7"/>
       <c r="D26" s="8"/>
       <c r="E26" s="8"/>
@@ -1550,8 +1550,8 @@
       <c r="H26" s="13"/>
     </row>
     <row r="27" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="34"/>
-      <c r="B27" s="35"/>
+      <c r="A27" s="83"/>
+      <c r="B27" s="84"/>
       <c r="C27" s="10"/>
       <c r="D27" s="11"/>
       <c r="E27" s="11"/>
@@ -1560,84 +1560,84 @@
       <c r="H27" s="16"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="62" t="s">
+      <c r="A28" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
       <c r="E28" s="8"/>
       <c r="F28" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G28" s="68" t="s">
+      <c r="G28" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="H28" s="70" t="s">
+      <c r="H28" s="50" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="62"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
+      <c r="A29" s="42"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
       <c r="F29" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="G29" s="69"/>
-      <c r="H29" s="71"/>
+      <c r="G29" s="49"/>
+      <c r="H29" s="51"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="62"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
-      <c r="H30" s="64"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
+      <c r="G30" s="43"/>
+      <c r="H30" s="44"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="62"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
-      <c r="H31" s="64"/>
+      <c r="A31" s="42"/>
+      <c r="B31" s="43"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
+      <c r="G31" s="43"/>
+      <c r="H31" s="44"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="62"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="64"/>
+      <c r="A32" s="42"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="44"/>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="62"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="64"/>
+      <c r="A33" s="42"/>
+      <c r="B33" s="43"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
+      <c r="G33" s="43"/>
+      <c r="H33" s="44"/>
     </row>
     <row r="34" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="65"/>
-      <c r="B34" s="66"/>
-      <c r="C34" s="66"/>
-      <c r="D34" s="66"/>
-      <c r="E34" s="66"/>
-      <c r="F34" s="66"/>
-      <c r="G34" s="66"/>
-      <c r="H34" s="67"/>
+      <c r="A34" s="45"/>
+      <c r="B34" s="46"/>
+      <c r="C34" s="46"/>
+      <c r="D34" s="46"/>
+      <c r="E34" s="46"/>
+      <c r="F34" s="46"/>
+      <c r="G34" s="46"/>
+      <c r="H34" s="47"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="25" t="s">
@@ -1865,11 +1865,15 @@
     </row>
   </sheetData>
   <mergeCells count="39">
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="E3:H4"/>
-    <mergeCell ref="A28:D28"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A29:E29"/>
     <mergeCell ref="A30:H34"/>
     <mergeCell ref="G28:G29"/>
@@ -1884,17 +1888,13 @@
     <mergeCell ref="A8:B9"/>
     <mergeCell ref="F8:F9"/>
     <mergeCell ref="C8:E9"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:B13"/>
     <mergeCell ref="A14:B14"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="A3:D3"/>
     <mergeCell ref="A24:B24"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="E3:H4"/>
+    <mergeCell ref="A28:D28"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:B27"/>

</xml_diff>